<commit_message>
rm landsat if scale10-20m
</commit_message>
<xml_diff>
--- a/windowsize/windowsize.xlsx
+++ b/windowsize/windowsize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuna\Documents\GitHub\PhD\Remote-Sensing-of-Albedo\windowsize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\Remote-Sensing-of-Albedo\windowsize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBE0701-F398-427A-8CB4-17788A9F9271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA19C753-51AA-4F8E-BB0B-0B66162C551B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22788" yWindow="1296" windowWidth="21600" windowHeight="11292" activeTab="3" xr2:uid="{B232E844-3A6C-4B6B-A9EB-18E9F8654100}"/>
+    <workbookView xWindow="13065" yWindow="2400" windowWidth="22590" windowHeight="15375" xr2:uid="{B232E844-3A6C-4B6B-A9EB-18E9F8654100}"/>
   </bookViews>
   <sheets>
     <sheet name="KAN" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>AWS</t>
   </si>
@@ -157,6 +157,36 @@
   </si>
   <si>
     <t>NSEM</t>
+  </si>
+  <si>
+    <t>NSE(log)</t>
+  </si>
+  <si>
+    <r>
+      <t>0.9919</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.0155</t>
+    </r>
+  </si>
+  <si>
+    <t>0.9786±0.0162</t>
   </si>
 </sst>
 </file>
@@ -207,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,6 +264,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,7 +327,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -371,10 +407,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.79</c:v>
@@ -464,7 +500,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1180012095"/>
@@ -526,7 +562,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1180016255"/>
@@ -574,7 +610,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1145,13 +1181,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -1481,34 +1517,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2B38F3-0AD8-47D2-9D5C-8483ADF7421C}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2183,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CF6377-C578-4FF4-8956-4ADE9C75F591}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2230,7 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2219,72 +2255,81 @@
       <c r="H1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10</v>
       </c>
       <c r="B2" s="3">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D2" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>-1.9E-3</v>
       </c>
       <c r="E2" s="4">
-        <v>0.1072</v>
+        <v>0.122</v>
       </c>
       <c r="F2" s="4">
-        <v>4.5999999999999999E-3</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="G2" s="4">
-        <v>0.62900190164238401</v>
+        <v>0.58350000000000002</v>
       </c>
       <c r="H2" s="4">
-        <v>0.88167675377210397</v>
+        <v>0.85409999999999997</v>
       </c>
       <c r="I2" s="4">
-        <v>0.42493126110576201</v>
-      </c>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.58889999999999998</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.3866</v>
+      </c>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20</v>
       </c>
       <c r="B3" s="3">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4">
-        <v>2.9600000000000001E-2</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="E3" s="4">
-        <v>0.1095</v>
+        <v>0.12540000000000001</v>
       </c>
       <c r="F3" s="4">
-        <v>4.5999999999999999E-3</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="G3" s="4">
-        <v>0.61131404375961895</v>
+        <v>0.55679999999999996</v>
       </c>
       <c r="H3" s="4">
-        <v>0.87539624945765804</v>
+        <v>0.84279999999999999</v>
       </c>
       <c r="I3" s="4">
-        <v>0.416379813410377</v>
-      </c>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.56689999999999996</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.37280000000000002</v>
+      </c>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -2310,11 +2355,14 @@
         <v>0.87604601656874403</v>
       </c>
       <c r="I4" s="4">
+        <v>0.60950453109122305</v>
+      </c>
+      <c r="J4" s="4">
         <v>0.42071543139873702</v>
       </c>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -2340,11 +2388,14 @@
         <v>0.87500877672319299</v>
       </c>
       <c r="I5" s="4">
+        <v>0.60221042743398001</v>
+      </c>
+      <c r="J5" s="4">
         <v>0.420694231545029</v>
       </c>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>90</v>
       </c>
@@ -2370,11 +2421,14 @@
         <v>0.87605608246177002</v>
       </c>
       <c r="I6" s="4">
+        <v>0.60787170266822999</v>
+      </c>
+      <c r="J6" s="4">
         <v>0.43179692597735297</v>
       </c>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>150</v>
       </c>
@@ -2400,9 +2454,108 @@
         <v>0.85655535961954998</v>
       </c>
       <c r="I7" s="4">
+        <v>0.583177321848107</v>
+      </c>
+      <c r="J7" s="4">
         <v>0.39185647900051002</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.1072</v>
+      </c>
+      <c r="F17" s="4">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.62900190164238401</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.88167675377210397</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.61262844431324703</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.42493126110576201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.1095</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.61131404375961895</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.87539624945765804</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.59774741917962604</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.416379813410377</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>